<commit_message>
access excel row with header name
</commit_message>
<xml_diff>
--- a/cypress/fixtures/ab.xlsx
+++ b/cypress/fixtures/ab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB\Desktop\cypress\qa-cypress-project\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C051F8E4-291D-4BF1-AFAB-9DD7E1C81D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E3522F-A1F4-41F8-BA3B-EB93BBE62AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{D160F7D0-5E65-46F8-B3AB-F5247FD7B081}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -42,9 +42,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
     <t>pass1</t>
   </si>
   <si>
@@ -58,6 +55,12 @@
   </si>
   <si>
     <t>pass3</t>
+  </si>
+  <si>
+    <t>"user1"</t>
+  </si>
+  <si>
+    <t>expected</t>
   </si>
 </sst>
 </file>
@@ -409,44 +412,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74076BED-F7D1-4855-B82F-8F6AA51A5484}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B4" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>